<commit_message>
Actualizaciones en la practica 4
</commit_message>
<xml_diff>
--- a/practicas_resueltas/diagramas_de_gantt/ejercicio_10_tp4.xlsx
+++ b/practicas_resueltas/diagramas_de_gantt/ejercicio_10_tp4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="39">
   <si>
     <t>LLEGADA</t>
   </si>
@@ -95,9 +95,6 @@
     <t>FCFS</t>
   </si>
   <si>
-    <t>I/O</t>
-  </si>
-  <si>
     <t>(R1, 2, 1)</t>
   </si>
   <si>
@@ -120,6 +117,30 @@
   </si>
   <si>
     <t>R3</t>
+  </si>
+  <si>
+    <t>RR TV (Q = 2)</t>
+  </si>
+  <si>
+    <t>(R1, 2, 3) (R1, 3, 2)</t>
+  </si>
+  <si>
+    <t>(R2, 3, 2)</t>
+  </si>
+  <si>
+    <t>(R2, 2, 3)</t>
+  </si>
+  <si>
+    <t>(R1, 1, 2)</t>
+  </si>
+  <si>
+    <t>I/O (rec, ins, dur)</t>
+  </si>
+  <si>
+    <t>ER1</t>
+  </si>
+  <si>
+    <t>ER2</t>
   </si>
 </sst>
 </file>
@@ -143,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,9 +376,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -405,6 +429,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AD23"/>
+  <dimension ref="B2:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="59" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -800,26 +839,26 @@
         <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="24">
-        <v>2</v>
-      </c>
-      <c r="I3" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24">
-        <v>3</v>
-      </c>
-      <c r="M3" s="24" t="s">
+      <c r="H3" s="23">
+        <v>2</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23">
+        <v>3</v>
+      </c>
+      <c r="M3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="9"/>
@@ -834,7 +873,7 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
-      <c r="Z3" s="16"/>
+      <c r="Z3" s="15"/>
       <c r="AA3" s="9"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8">
@@ -855,44 +894,42 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="20" t="s">
         <v>25</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="26">
-        <v>2</v>
-      </c>
-      <c r="K4" s="27">
-        <v>3</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26">
-        <v>4</v>
-      </c>
-      <c r="S4" s="26">
+      <c r="J4" s="25">
+        <v>2</v>
+      </c>
+      <c r="K4" s="26"/>
+      <c r="L4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25">
+        <v>4</v>
+      </c>
+      <c r="S4" s="25">
         <v>5</v>
       </c>
-      <c r="T4" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26" t="s">
+      <c r="T4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25" t="s">
         <v>8</v>
       </c>
       <c r="X4" s="9"/>
@@ -918,30 +955,30 @@
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28">
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27">
         <v>1</v>
       </c>
-      <c r="O5" s="28">
-        <v>2</v>
-      </c>
-      <c r="P5" s="28">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="28" t="s">
+      <c r="O5" s="27">
+        <v>2</v>
+      </c>
+      <c r="P5" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="27" t="s">
         <v>6</v>
       </c>
       <c r="R5" s="9"/>
@@ -973,46 +1010,46 @@
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>27</v>
       </c>
       <c r="G6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25">
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24">
         <v>1</v>
       </c>
-      <c r="U6" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="V6" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25">
-        <v>2</v>
-      </c>
-      <c r="Y6" s="25">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA6" s="25">
-        <v>4</v>
-      </c>
-      <c r="AB6" s="29" t="s">
+      <c r="U6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="24">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA6" s="24">
+        <v>4</v>
+      </c>
+      <c r="AB6" s="28" t="s">
         <v>9</v>
       </c>
       <c r="AC6" s="8">
@@ -1033,10 +1070,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -1046,18 +1083,18 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="30" t="s">
+      <c r="O7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30">
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29">
         <v>1</v>
       </c>
-      <c r="V7" s="30" t="s">
+      <c r="V7" s="29" t="s">
         <v>10</v>
       </c>
       <c r="W7" s="11"/>
@@ -1074,9 +1111,9 @@
       </c>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1119,7 +1156,7 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
-      <c r="AB8" s="18"/>
+      <c r="AB8" s="17"/>
       <c r="AC8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1128,9 +1165,9 @@
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1157,12 +1194,12 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
-      <c r="AB9" s="18"/>
-      <c r="AC9" s="15">
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="14">
         <f>AVERAGE(AC3:AC8)</f>
         <v>10.8</v>
       </c>
-      <c r="AD9" s="31">
+      <c r="AD9" s="30">
         <f>AVERAGE(AD3:AD8)</f>
         <v>6.6</v>
       </c>
@@ -1194,9 +1231,9 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="17"/>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="F11" s="1" t="s">
@@ -1225,13 +1262,13 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
-      <c r="Z11" s="19"/>
+      <c r="Z11" s="18"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="17"/>
+      <c r="AB11" s="16"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -1243,7 +1280,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -1305,9 +1342,11 @@
       <c r="Z14" s="3">
         <v>19</v>
       </c>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3">
+      <c r="AA14" s="3">
         <v>20</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>21</v>
       </c>
       <c r="AC14" s="4" t="s">
         <v>3</v>
@@ -1327,22 +1366,32 @@
         <v>4</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="23">
+        <v>2</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23">
+        <v>3</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>6</v>
+      </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
-      <c r="Q15" s="32"/>
+      <c r="Q15" s="31"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
       <c r="T15" s="9"/>
@@ -1351,11 +1400,15 @@
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
-      <c r="Z15" s="16"/>
+      <c r="Z15" s="15"/>
       <c r="AA15" s="9"/>
       <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="7"/>
+      <c r="AC15" s="8">
+        <v>6</v>
+      </c>
+      <c r="AD15" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
@@ -1368,35 +1421,57 @@
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="20" t="s">
         <v>25</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
+      <c r="I16" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="25">
+        <v>2</v>
+      </c>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25">
+        <v>3</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25">
+        <v>4</v>
+      </c>
+      <c r="V16" s="25">
+        <v>5</v>
+      </c>
+      <c r="W16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="X16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y16" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="7"/>
+      <c r="AC16" s="8">
+        <v>17</v>
+      </c>
+      <c r="AD16" s="7">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
@@ -1409,23 +1484,33 @@
         <v>4</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="J17" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27">
+        <v>1</v>
+      </c>
+      <c r="N17" s="27">
+        <v>2</v>
+      </c>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27">
+        <v>3</v>
+      </c>
+      <c r="R17" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
@@ -1436,8 +1521,12 @@
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
       <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="7"/>
+      <c r="AC17" s="8">
+        <v>9</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
@@ -1450,10 +1539,10 @@
         <v>5</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>27</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
@@ -1461,24 +1550,46 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
+      <c r="M18" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24">
+        <v>2</v>
+      </c>
+      <c r="X18" s="24">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z18" s="24">
+        <v>4</v>
+      </c>
+      <c r="AA18" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="AB18" s="8"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="7"/>
+      <c r="AC18" s="8">
+        <v>15</v>
+      </c>
+      <c r="AD18" s="7">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
@@ -1491,10 +1602,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -1504,12 +1615,18 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
+      <c r="O19" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29">
+        <v>1</v>
+      </c>
+      <c r="T19" s="29" t="s">
+        <v>10</v>
+      </c>
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11"/>
@@ -1518,28 +1635,56 @@
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
       <c r="AB19" s="12"/>
-      <c r="AC19" s="12"/>
-      <c r="AD19" s="7"/>
+      <c r="AC19" s="12">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
       <c r="F20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
@@ -1549,7 +1694,7 @@
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
-      <c r="AB20" s="18"/>
+      <c r="AB20" s="17"/>
       <c r="AC20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1558,13 +1703,15 @@
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -1585,16 +1732,26 @@
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
-      <c r="AB21" s="18"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="13"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="14">
+        <f>AVERAGE(AC15:AC20)</f>
+        <v>10.6</v>
+      </c>
+      <c r="AD21" s="30">
+        <f>AVERAGE(AD15:AD20)</f>
+        <v>6.4</v>
+      </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -1612,16 +1769,20 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
+      <c r="AB22" s="17"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -1639,9 +1800,1470 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
-      <c r="Z23" s="19"/>
+      <c r="Z23" s="18"/>
       <c r="AA23" s="10"/>
-      <c r="AB23" s="17"/>
+      <c r="AB23" s="16"/>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>3</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4</v>
+      </c>
+      <c r="L26" s="3">
+        <v>5</v>
+      </c>
+      <c r="M26" s="3">
+        <v>6</v>
+      </c>
+      <c r="N26" s="3">
+        <v>7</v>
+      </c>
+      <c r="O26" s="3">
+        <v>8</v>
+      </c>
+      <c r="P26" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>10</v>
+      </c>
+      <c r="R26" s="3">
+        <v>11</v>
+      </c>
+      <c r="S26" s="3">
+        <v>12</v>
+      </c>
+      <c r="T26" s="3">
+        <v>13</v>
+      </c>
+      <c r="U26" s="3">
+        <v>14</v>
+      </c>
+      <c r="V26" s="3">
+        <v>15</v>
+      </c>
+      <c r="W26" s="3">
+        <v>16</v>
+      </c>
+      <c r="X26" s="3">
+        <v>17</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>18</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>19</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>21</v>
+      </c>
+      <c r="AC26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="23">
+        <v>2</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23">
+        <v>3</v>
+      </c>
+      <c r="O27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="33"/>
+      <c r="Z27" s="33"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="7">
+        <v>15</v>
+      </c>
+      <c r="AD27" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="25">
+        <v>2</v>
+      </c>
+      <c r="K28" s="25">
+        <v>3</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="25">
+        <v>5</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="S28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="33"/>
+      <c r="Z28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="7">
+        <v>10</v>
+      </c>
+      <c r="AD28" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>3</v>
+      </c>
+      <c r="C29" s="5">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5">
+        <v>4</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27">
+        <v>1</v>
+      </c>
+      <c r="M29" s="27">
+        <v>2</v>
+      </c>
+      <c r="N29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27">
+        <v>3</v>
+      </c>
+      <c r="W29" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="X29" s="33"/>
+      <c r="Y29" s="33"/>
+      <c r="Z29" s="33"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="33"/>
+      <c r="AC29" s="7">
+        <v>14</v>
+      </c>
+      <c r="AD29" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>4</v>
+      </c>
+      <c r="C30" s="5">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5">
+        <v>5</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24">
+        <v>1</v>
+      </c>
+      <c r="P30" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="R30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="S30" s="24"/>
+      <c r="T30" s="24"/>
+      <c r="U30" s="24"/>
+      <c r="V30" s="24"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24">
+        <v>2</v>
+      </c>
+      <c r="Y30" s="24">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="24">
+        <v>4</v>
+      </c>
+      <c r="AA30" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="7">
+        <v>15</v>
+      </c>
+      <c r="AD30" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5">
+        <v>8</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29">
+        <v>1</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="34">
+        <v>6</v>
+      </c>
+      <c r="AD31" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="M32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="V33" s="18"/>
+      <c r="W33" s="18"/>
+      <c r="X33" s="18"/>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="18"/>
+      <c r="AA33" s="18"/>
+      <c r="AB33" s="32"/>
+      <c r="AC33" s="36">
+        <f>AVERAGE(AC27:AC32)</f>
+        <v>12</v>
+      </c>
+      <c r="AD33" s="36">
+        <f>AVERAGE(AD27:AD32)</f>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="13"/>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3">
+        <v>2</v>
+      </c>
+      <c r="J37" s="3">
+        <v>3</v>
+      </c>
+      <c r="K37" s="3">
+        <v>4</v>
+      </c>
+      <c r="L37" s="3">
+        <v>5</v>
+      </c>
+      <c r="M37" s="3">
+        <v>6</v>
+      </c>
+      <c r="N37" s="3">
+        <v>7</v>
+      </c>
+      <c r="O37" s="3">
+        <v>8</v>
+      </c>
+      <c r="P37" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>10</v>
+      </c>
+      <c r="R37" s="3">
+        <v>11</v>
+      </c>
+      <c r="S37" s="3">
+        <v>12</v>
+      </c>
+      <c r="T37" s="3">
+        <v>13</v>
+      </c>
+      <c r="U37" s="3">
+        <v>14</v>
+      </c>
+      <c r="V37" s="3">
+        <v>15</v>
+      </c>
+      <c r="W37" s="3">
+        <v>16</v>
+      </c>
+      <c r="X37" s="3">
+        <v>17</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>18</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>19</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>21</v>
+      </c>
+      <c r="AC37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD37" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="23">
+        <v>2</v>
+      </c>
+      <c r="I38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23">
+        <v>3</v>
+      </c>
+      <c r="O38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="U38" s="33"/>
+      <c r="V38" s="33"/>
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+      <c r="Y38" s="33"/>
+      <c r="Z38" s="33"/>
+      <c r="AA38" s="33"/>
+      <c r="AB38" s="33"/>
+      <c r="AC38" s="7">
+        <v>14</v>
+      </c>
+      <c r="AD38" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B39" s="5">
+        <v>2</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2</v>
+      </c>
+      <c r="D39" s="5">
+        <v>6</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="25">
+        <v>2</v>
+      </c>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25">
+        <v>3</v>
+      </c>
+      <c r="N39" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="O39" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="P39" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q39" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25">
+        <v>4</v>
+      </c>
+      <c r="V39" s="25">
+        <v>5</v>
+      </c>
+      <c r="W39" s="25"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z39" s="33"/>
+      <c r="AA39" s="33"/>
+      <c r="AB39" s="33"/>
+      <c r="AC39" s="7">
+        <v>17</v>
+      </c>
+      <c r="AD39" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B40" s="5">
+        <v>3</v>
+      </c>
+      <c r="C40" s="5">
+        <v>3</v>
+      </c>
+      <c r="D40" s="5">
+        <v>4</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="27">
+        <v>1</v>
+      </c>
+      <c r="L40" s="27">
+        <v>2</v>
+      </c>
+      <c r="M40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="O40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27">
+        <v>3</v>
+      </c>
+      <c r="S40" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="T40" s="33"/>
+      <c r="U40" s="33"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
+      <c r="Y40" s="33"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="33"/>
+      <c r="AB40" s="33"/>
+      <c r="AC40" s="7">
+        <v>10</v>
+      </c>
+      <c r="AD40" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B41" s="5">
+        <v>4</v>
+      </c>
+      <c r="C41" s="5">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24">
+        <v>1</v>
+      </c>
+      <c r="P41" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q41" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="R41" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24">
+        <v>2</v>
+      </c>
+      <c r="X41" s="24">
+        <v>3</v>
+      </c>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="24">
+        <v>4</v>
+      </c>
+      <c r="AA41" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB41" s="33"/>
+      <c r="AC41" s="7">
+        <v>15</v>
+      </c>
+      <c r="AD41" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B42" s="5">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5">
+        <v>8</v>
+      </c>
+      <c r="D42" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="P42" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="10"/>
+      <c r="AC42" s="34">
+        <v>3</v>
+      </c>
+      <c r="AD42" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q43" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="R43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="S43" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="T43" s="18"/>
+      <c r="U43" s="18"/>
+      <c r="V43" s="18"/>
+      <c r="W43" s="18"/>
+      <c r="X43" s="18"/>
+      <c r="Y43" s="18"/>
+      <c r="Z43" s="18"/>
+      <c r="AA43" s="18"/>
+      <c r="AB43" s="32"/>
+      <c r="AC43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+      <c r="V44" s="18"/>
+      <c r="W44" s="18"/>
+      <c r="X44" s="18"/>
+      <c r="Y44" s="18"/>
+      <c r="Z44" s="18"/>
+      <c r="AA44" s="18"/>
+      <c r="AB44" s="32"/>
+      <c r="AC44" s="36">
+        <f>AVERAGE(AC38:AC43)</f>
+        <v>11.8</v>
+      </c>
+      <c r="AD44" s="36">
+        <f>AVERAGE(AD38:AD43)</f>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
+      <c r="W45" s="10"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="10"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="13"/>
+    </row>
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="3">
+        <v>2</v>
+      </c>
+      <c r="J48" s="3">
+        <v>3</v>
+      </c>
+      <c r="K48" s="3">
+        <v>4</v>
+      </c>
+      <c r="L48" s="3">
+        <v>5</v>
+      </c>
+      <c r="M48" s="3">
+        <v>6</v>
+      </c>
+      <c r="N48" s="3">
+        <v>7</v>
+      </c>
+      <c r="O48" s="3">
+        <v>8</v>
+      </c>
+      <c r="P48" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>10</v>
+      </c>
+      <c r="R48" s="3">
+        <v>11</v>
+      </c>
+      <c r="S48" s="3">
+        <v>12</v>
+      </c>
+      <c r="T48" s="3">
+        <v>13</v>
+      </c>
+      <c r="U48" s="3">
+        <v>14</v>
+      </c>
+      <c r="V48" s="3">
+        <v>15</v>
+      </c>
+      <c r="W48" s="3">
+        <v>16</v>
+      </c>
+      <c r="X48" s="3">
+        <v>17</v>
+      </c>
+      <c r="Y48" s="3">
+        <v>18</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>19</v>
+      </c>
+      <c r="AA48" s="3">
+        <v>20</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>21</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD48" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5">
+        <v>4</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="33"/>
+      <c r="S49" s="33"/>
+      <c r="T49" s="33"/>
+      <c r="U49" s="33"/>
+      <c r="V49" s="33"/>
+      <c r="W49" s="33"/>
+      <c r="X49" s="33"/>
+      <c r="Y49" s="33"/>
+      <c r="Z49" s="33"/>
+      <c r="AA49" s="33"/>
+      <c r="AB49" s="33"/>
+      <c r="AC49" s="7"/>
+      <c r="AD49" s="8"/>
+    </row>
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
+        <v>2</v>
+      </c>
+      <c r="C50" s="5">
+        <v>2</v>
+      </c>
+      <c r="D50" s="5">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="33"/>
+      <c r="S50" s="33"/>
+      <c r="T50" s="33"/>
+      <c r="U50" s="33"/>
+      <c r="V50" s="33"/>
+      <c r="W50" s="33"/>
+      <c r="X50" s="33"/>
+      <c r="Y50" s="33"/>
+      <c r="Z50" s="33"/>
+      <c r="AA50" s="33"/>
+      <c r="AB50" s="33"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="8"/>
+    </row>
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
+        <v>3</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5">
+        <v>4</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="33"/>
+      <c r="S51" s="33"/>
+      <c r="T51" s="33"/>
+      <c r="U51" s="33"/>
+      <c r="V51" s="33"/>
+      <c r="W51" s="33"/>
+      <c r="X51" s="33"/>
+      <c r="Y51" s="33"/>
+      <c r="Z51" s="33"/>
+      <c r="AA51" s="33"/>
+      <c r="AB51" s="33"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="8"/>
+    </row>
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>4</v>
+      </c>
+      <c r="C52" s="5">
+        <v>6</v>
+      </c>
+      <c r="D52" s="5">
+        <v>5</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="33"/>
+      <c r="S52" s="33"/>
+      <c r="T52" s="33"/>
+      <c r="U52" s="33"/>
+      <c r="V52" s="33"/>
+      <c r="W52" s="33"/>
+      <c r="X52" s="33"/>
+      <c r="Y52" s="33"/>
+      <c r="Z52" s="33"/>
+      <c r="AA52" s="33"/>
+      <c r="AB52" s="33"/>
+      <c r="AC52" s="7"/>
+      <c r="AD52" s="8"/>
+    </row>
+    <row r="53" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>5</v>
+      </c>
+      <c r="C53" s="5">
+        <v>8</v>
+      </c>
+      <c r="D53" s="5">
+        <v>2</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="10"/>
+      <c r="V53" s="10"/>
+      <c r="W53" s="10"/>
+      <c r="X53" s="10"/>
+      <c r="Y53" s="10"/>
+      <c r="Z53" s="10"/>
+      <c r="AA53" s="10"/>
+      <c r="AB53" s="10"/>
+      <c r="AC53" s="34"/>
+      <c r="AD53" s="12"/>
+    </row>
+    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="18"/>
+      <c r="U54" s="18"/>
+      <c r="V54" s="18"/>
+      <c r="W54" s="18"/>
+      <c r="X54" s="18"/>
+      <c r="Y54" s="18"/>
+      <c r="Z54" s="18"/>
+      <c r="AA54" s="18"/>
+      <c r="AB54" s="32"/>
+      <c r="AC54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="18"/>
+      <c r="U55" s="18"/>
+      <c r="V55" s="18"/>
+      <c r="W55" s="18"/>
+      <c r="X55" s="18"/>
+      <c r="Y55" s="18"/>
+      <c r="Z55" s="18"/>
+      <c r="AA55" s="18"/>
+      <c r="AB55" s="32"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
+    </row>
+    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10"/>
+      <c r="V56" s="10"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="10"/>
+      <c r="Y56" s="10"/>
+      <c r="Z56" s="10"/>
+      <c r="AA56" s="10"/>
+      <c r="AB56" s="12"/>
+      <c r="AC56" s="13"/>
+      <c r="AD56" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>